<commit_message>
Location card templates, plus mixed tribe creatures
</commit_message>
<xml_diff>
--- a/src/components/Proxy Data Battlegear.xlsx
+++ b/src/components/Proxy Data Battlegear.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bulba\Documents\GitHub\chaotic-react\src\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A1C1C6-94DA-442D-A7EC-BB052678BB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB18D36E-CFA5-4713-8731-FA4977144533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="5745" windowWidth="19185" windowHeight="11985" xr2:uid="{7869EBB4-B98F-4E46-A90F-0E408BD70E81}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{7869EBB4-B98F-4E46-A90F-0E408BD70E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="717">
   <si>
     <t>Name</t>
   </si>
@@ -2226,6 +2226,67 @@
   </si>
   <si>
     <t>Equipped Creature has "Expend :earth:earth: Gain 50 :courage:Courage."</t>
+  </si>
+  <si>
+    <t>Giant Mechanical Python of Pyrithion</t>
+  </si>
+  <si>
+    <t>"It's indestructible made by Ulmar." - Pyrithion</t>
+  </si>
+  <si>
+    <t>https://imgur.com/MVu1yUi</t>
+  </si>
+  <si>
+    <t>Chaor's Battle Titan Statue</t>
+  </si>
+  <si>
+    <t>https://imgur.com/jAQIbeg</t>
+  </si>
+  <si>
+    <t>https://imgur.com/YMi84KC</t>
+  </si>
+  <si>
+    <t>Chaor's Mugic Battle Axe</t>
+  </si>
+  <si>
+    <t>https://imgur.com/0w0Fs2q</t>
+  </si>
+  <si>
+    <t>https://imgur.com/MVu1yUi.png</t>
+  </si>
+  <si>
+    <t>https://imgur.com/jAQIbeg.png</t>
+  </si>
+  <si>
+    <t>https://imgur.com/YMi84KC.png</t>
+  </si>
+  <si>
+    <t>https://imgur.com/0w0Fs2q.png</t>
+  </si>
+  <si>
+    <t>The Staff Belonged to the Father of Vitog. Vertog</t>
+  </si>
+  <si>
+    <t>Staff of Ar'Khan From Spiritlands</t>
+  </si>
+  <si>
+    <t>Returns one attack back to the opposing Creature and returns one attack by battlegear; back to the opposing Creature. Once every Battle.
+If user takes 25 or more damage, destroy this.</t>
+  </si>
+  <si>
+    <t>Recklessness 10
+Increase :fire:Fire attacks by 20.</t>
+  </si>
+  <si>
+    <t>Increase Energy by 20
+Increase :fire:Fire attacks by 5
+Increase Mugic attacks by 5</t>
+  </si>
+  <si>
+    <t>Increase Energy by 50
+Increase :fire:Fire attacks by 10
+Increase :speed:Speed by 50
+Only Chaor or Ulmar can be equipped with this Battlegear.</t>
   </si>
 </sst>
 </file>
@@ -2669,17 +2730,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7629AE8-A5B6-45B9-9607-CE7C7885BD97}">
-  <dimension ref="A1:K159"/>
+  <dimension ref="A1:V163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E122" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="181.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6293,7 +6354,7 @@
         <v>https://i.imgur.com/ZrJWgvE.png</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>395</v>
       </c>
@@ -6317,7 +6378,7 @@
         <v>https://i.imgur.com/6XebUsF.png</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>397</v>
       </c>
@@ -6341,7 +6402,7 @@
         <v>https://i.imgur.com/M8eHgQ1.png</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>400</v>
       </c>
@@ -6365,7 +6426,7 @@
         <v>https://i.imgur.com/RtzNzRk.png</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>403</v>
       </c>
@@ -6389,7 +6450,7 @@
         <v>https://i.imgur.com/hAW6uww.png</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>405</v>
       </c>
@@ -6416,7 +6477,7 @@
         <v>https://i.imgur.com/SNW93Vm.png</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>408</v>
       </c>
@@ -6440,7 +6501,7 @@
         <v>https://i.imgur.com/I4969fD.png</v>
       </c>
     </row>
-    <row r="151" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>29</v>
       </c>
@@ -6464,7 +6525,7 @@
         <v>https://i.imgur.com/aKVIkOT.png</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>52</v>
       </c>
@@ -6488,7 +6549,7 @@
         <v>https://i.imgur.com/dYMVHMP.png</v>
       </c>
     </row>
-    <row r="153" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>83</v>
       </c>
@@ -6512,7 +6573,7 @@
         <v>https://i.imgur.com/ciQOuJV.png</v>
       </c>
     </row>
-    <row r="154" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>417</v>
       </c>
@@ -6536,7 +6597,7 @@
         <v>https://i.imgur.com/X47rwXo.png</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>420</v>
       </c>
@@ -6560,7 +6621,7 @@
         <v>https://i.imgur.com/VMXktou.png</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>422</v>
       </c>
@@ -6587,7 +6648,7 @@
         <v>https://i.imgur.com/F23ZOlY.png</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>424</v>
       </c>
@@ -6611,7 +6672,7 @@
         <v>https://i.imgur.com/pS5B3uR.png</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>426</v>
       </c>
@@ -6641,7 +6702,7 @@
         <v>https://i.imgur.com/vquBcPw.png</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>431</v>
       </c>
@@ -6669,6 +6730,92 @@
       <c r="I159" t="str">
         <f>VLOOKUP(A159,Sheet2!$A$1:$B$158,2,FALSE)</f>
         <v>https://i.imgur.com/2wwoh4t.png</v>
+      </c>
+    </row>
+    <row r="160" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E160" s="4" t="s">
+        <v>714</v>
+      </c>
+      <c r="F160" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="I160" s="6" t="s">
+        <v>707</v>
+      </c>
+      <c r="V160" s="5" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="161" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E161" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="I161" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="V161" s="5" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="162" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E162" s="4" t="s">
+        <v>713</v>
+      </c>
+      <c r="F162" t="s">
+        <v>711</v>
+      </c>
+      <c r="I162" s="6" t="s">
+        <v>709</v>
+      </c>
+      <c r="V162" s="5" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="163" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E163" s="4" t="s">
+        <v>715</v>
+      </c>
+      <c r="I163" s="6" t="s">
+        <v>710</v>
+      </c>
+      <c r="V163" s="5" t="s">
+        <v>706</v>
       </c>
     </row>
   </sheetData>
@@ -6677,6 +6824,12 @@
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="I160" r:id="rId1" xr:uid="{33DB7C8B-23B7-40A8-9A78-C5DA4FCEE44F}"/>
+    <hyperlink ref="I161" r:id="rId2" xr:uid="{9F6436F1-DDC6-403C-A5EA-EC91C2CC6AC0}"/>
+    <hyperlink ref="I162" r:id="rId3" xr:uid="{ADD59FB4-9EE9-4D70-A39D-317B6142F80F}"/>
+    <hyperlink ref="I163" r:id="rId4" xr:uid="{EE3AD271-4998-4CCC-B778-68E2EB1DC44E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>